<commit_message>
wrong report picture uploaded - fixed
</commit_message>
<xml_diff>
--- a/lab_2/Report.xlsx
+++ b/lab_2/Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shust\Desktop\AOP_cource\lab_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DF6B02-85A4-4D9A-8989-076A8A764969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B52381A-3A94-4BE4-B099-D80D5C990EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1290" yWindow="570" windowWidth="24870" windowHeight="15045" xr2:uid="{1F6D4EA5-1A38-4001-9514-C448F4ABEEB0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{1F6D4EA5-1A38-4001-9514-C448F4ABEEB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="56">
   <si>
     <t>p01</t>
   </si>
@@ -148,27 +148,6 @@
   </si>
   <si>
     <t>[1, 0, 0, 1, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 1, 1, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1, 1, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 0, 0, 0, 1]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1, 0, 0, 0, 1, 1, 1, 0, 0, 0, 1, 1, 1]</t>
   </si>
   <si>
     <t>[1, 1, 1, 1, 0, 0, 0, 0, 0, 0]</t>
@@ -451,15 +430,6 @@
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -484,15 +454,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -504,15 +465,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -539,6 +491,33 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -856,7 +835,7 @@
   <dimension ref="B1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,836 +851,836 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28"/>
-      <c r="C3" s="35" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="27" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>57</v>
+      <c r="C7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>56</v>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="28"/>
-      <c r="C11" s="35" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="35" t="s">
+      <c r="H11" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="I11" s="27" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="5">
         <v>1652</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="5">
         <v>132</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="5">
         <v>1142</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="5">
         <v>352</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="5">
         <v>834</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="5">
         <v>1192</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="6">
         <v>11252</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>7163</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="5">
         <v>502</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="5">
         <v>1708</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="5">
         <v>1400</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="5">
         <v>10875</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="5">
         <v>28735</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="6">
         <v>42641</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="5">
         <v>10</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="5">
         <v>5</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="5">
         <v>6</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="5">
         <v>7</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="5">
         <v>8</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="5">
         <v>7</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="6">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="5">
         <v>10</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="5">
         <v>5</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="5">
         <v>6</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="5">
         <v>7</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="5">
         <v>8</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="5">
         <v>7</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="6">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <v>26900</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="7">
         <v>5319</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="7">
         <v>7020</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="7">
         <v>9593</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="7">
         <v>9809</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="7">
         <v>11597</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="8">
         <v>44340</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="14"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="32"/>
     </row>
     <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="28"/>
-      <c r="C19" s="33" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="25" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="15" t="s">
+      <c r="C22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="H22" s="15" t="s">
+      <c r="E22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="16" t="s">
-        <v>49</v>
+      <c r="I22" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>44</v>
+      <c r="C23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H24" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="21"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="35"/>
     </row>
     <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="28"/>
-      <c r="C27" s="26" t="s">
+      <c r="B27" s="19"/>
+      <c r="C27" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="26" t="s">
+      <c r="H27" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I27" s="27" t="s">
+      <c r="I27" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="13">
         <v>309</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="13">
         <v>51</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="13">
         <v>150</v>
       </c>
-      <c r="F28" s="22">
+      <c r="F28" s="13">
         <v>107</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G28" s="13">
         <v>900</v>
       </c>
-      <c r="H28" s="22">
+      <c r="H28" s="13">
         <v>1735</v>
       </c>
-      <c r="I28" s="23">
+      <c r="I28" s="14">
         <v>1458</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="13">
         <v>309</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="13">
         <v>47</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="13">
         <v>150</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="13">
         <v>107</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="13">
         <v>900</v>
       </c>
-      <c r="H29" s="22">
+      <c r="H29" s="13">
         <v>1735</v>
       </c>
-      <c r="I29" s="23">
+      <c r="I29" s="14">
         <v>1458</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="13">
         <v>266</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="13">
         <v>47</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="13">
         <v>146</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F30" s="13">
         <v>102</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G30" s="13">
         <v>888</v>
       </c>
-      <c r="H30" s="22">
+      <c r="H30" s="13">
         <v>1735</v>
       </c>
-      <c r="I30" s="23">
+      <c r="I30" s="14">
         <v>1441</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="13">
         <v>309</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="13">
         <v>51</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="13">
         <v>150</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="13">
         <v>107</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="13">
         <v>900</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H31" s="13">
         <v>1735</v>
       </c>
-      <c r="I31" s="23">
+      <c r="I31" s="14">
         <v>1458</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="15">
         <v>309</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="15">
         <v>47</v>
       </c>
-      <c r="E32" s="24">
+      <c r="E32" s="15">
         <v>150</v>
       </c>
-      <c r="F32" s="24">
+      <c r="F32" s="15">
         <v>107</v>
       </c>
-      <c r="G32" s="24">
+      <c r="G32" s="15">
         <v>900</v>
       </c>
-      <c r="H32" s="24">
+      <c r="H32" s="15">
         <v>1652</v>
       </c>
-      <c r="I32" s="25">
+      <c r="I32" s="16">
         <v>1458</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="21"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="35"/>
     </row>
     <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="28"/>
-      <c r="C35" s="26" t="s">
+      <c r="B35" s="19"/>
+      <c r="C35" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="26" t="s">
+      <c r="D35" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E35" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="26" t="s">
+      <c r="F35" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G35" s="26" t="s">
+      <c r="G35" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H35" s="26" t="s">
+      <c r="H35" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I35" s="27" t="s">
+      <c r="I35" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="22">
+      <c r="C36" s="13">
         <v>165</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="13">
         <v>23</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36" s="13">
         <v>190</v>
       </c>
-      <c r="F36" s="22">
+      <c r="F36" s="13">
         <v>50</v>
       </c>
-      <c r="G36" s="22">
+      <c r="G36" s="13">
         <v>104</v>
       </c>
-      <c r="H36" s="22">
+      <c r="H36" s="13">
         <v>160</v>
       </c>
-      <c r="I36" s="23">
+      <c r="I36" s="14">
         <v>749</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="22">
+      <c r="C37" s="13">
         <v>165</v>
       </c>
-      <c r="D37" s="22">
+      <c r="D37" s="13">
         <v>26</v>
       </c>
-      <c r="E37" s="22">
+      <c r="E37" s="13">
         <v>190</v>
       </c>
-      <c r="F37" s="22">
+      <c r="F37" s="13">
         <v>50</v>
       </c>
-      <c r="G37" s="22">
+      <c r="G37" s="13">
         <v>104</v>
       </c>
-      <c r="H37" s="22">
+      <c r="H37" s="13">
         <v>169</v>
       </c>
-      <c r="I37" s="23">
+      <c r="I37" s="14">
         <v>749</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="22">
+      <c r="C38" s="13">
         <v>127</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="13">
         <v>23</v>
       </c>
-      <c r="E38" s="22">
+      <c r="E38" s="13">
         <v>179</v>
       </c>
-      <c r="F38" s="22">
+      <c r="F38" s="13">
         <v>48</v>
       </c>
-      <c r="G38" s="22">
+      <c r="G38" s="13">
         <v>92</v>
       </c>
-      <c r="H38" s="22">
+      <c r="H38" s="13">
         <v>169</v>
       </c>
-      <c r="I38" s="23">
+      <c r="I38" s="14">
         <v>740</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="22">
+      <c r="C39" s="13">
         <v>165</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="13">
         <v>26</v>
       </c>
-      <c r="E39" s="22">
+      <c r="E39" s="13">
         <v>190</v>
       </c>
-      <c r="F39" s="22">
+      <c r="F39" s="13">
         <v>50</v>
       </c>
-      <c r="G39" s="22">
+      <c r="G39" s="13">
         <v>104</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H39" s="13">
         <v>169</v>
       </c>
-      <c r="I39" s="23">
+      <c r="I39" s="14">
         <v>749</v>
       </c>
     </row>
     <row r="40" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="24">
+      <c r="C40" s="15">
         <v>165</v>
       </c>
-      <c r="D40" s="24">
+      <c r="D40" s="15">
         <v>23</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E40" s="15">
         <v>190</v>
       </c>
-      <c r="F40" s="24">
+      <c r="F40" s="15">
         <v>50</v>
       </c>
-      <c r="G40" s="24">
+      <c r="G40" s="15">
         <v>104</v>
       </c>
-      <c r="H40" s="24">
+      <c r="H40" s="15">
         <v>160</v>
       </c>
-      <c r="I40" s="25">
+      <c r="I40" s="16">
         <v>749</v>
       </c>
     </row>

</xml_diff>